<commit_message>
Added feature to detect emotion while marking attendance and saving it in database .Also updated the Testcase for this feature.
</commit_message>
<xml_diff>
--- a/app/TestCases/Student/TestCase_Markattendance.xlsx
+++ b/app/TestCases/Student/TestCase_Markattendance.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB34641E-CD5B-4A1D-9DE1-6697E69314F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rehana\Desktop\Big_Data_Semester1\Programming_for_big-data\Project\FacialRecognitionAttendanceSystem\app\TestCases\Student\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85750469-A6F8-488A-8C90-1A8DE37FA95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -54,9 +59,6 @@
     <t xml:space="preserve">1. Open the attendance marking page. </t>
   </si>
   <si>
-    <t>The selected course should be displayed in the dropdown.</t>
-  </si>
-  <si>
     <t xml:space="preserve">2. Click on the course selection dropdown. </t>
   </si>
   <si>
@@ -72,9 +74,6 @@
     <t xml:space="preserve">1. Select a course from the course dropdown. </t>
   </si>
   <si>
-    <t>The session dropdown should populate with valid session values related to the selected course.</t>
-  </si>
-  <si>
     <t>2. Observe the session dropdown.</t>
   </si>
   <si>
@@ -102,9 +101,6 @@
     <t xml:space="preserve">1. Mark attendance for a student. </t>
   </si>
   <si>
-    <t>A validation error message should appear, indicating that duplicate attendance is not allowed for the same session.</t>
-  </si>
-  <si>
     <t>2. Attempt to mark attendance for the same student in the same session again.</t>
   </si>
   <si>
@@ -114,9 +110,6 @@
     <t>Verify Attendance Marking for Different Students</t>
   </si>
   <si>
-    <t>- Attendance should be successfully marked for each student.&amp;lt;br&amp;gt;- No duplicates should be allowed.</t>
-  </si>
-  <si>
     <t>TC06</t>
   </si>
   <si>
@@ -144,9 +137,6 @@
     <t xml:space="preserve">1. Try to mark attendance without selecting a course or session. </t>
   </si>
   <si>
-    <t xml:space="preserve"> Appropriate error messages should be displayed. The system should prevent invalid actions.</t>
-  </si>
-  <si>
     <t>2.. Try to mark attendance for an invalid session.</t>
   </si>
   <si>
@@ -160,13 +150,58 @@
   </si>
   <si>
     <t>The default course and session dropdowns should be empty. No attendance data should be displayed until a course and session are selected.</t>
+  </si>
+  <si>
+    <t>The selected course should be displayed in the dropdown.(Pass)</t>
+  </si>
+  <si>
+    <t>The session dropdown should populate with valid session values related to the selected course.(Pass)</t>
+  </si>
+  <si>
+    <t>(Pass)</t>
+  </si>
+  <si>
+    <t>A validation error message should appear, indicating that duplicate attendance is not allowed for the same session.(Pass)</t>
+  </si>
+  <si>
+    <t>Attendance should be successfully marked for each student. No duplicates should be allowed.(Pass)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Appropriate error messages should be displayed. The system should prevent invalid actions.(Pass)</t>
+  </si>
+  <si>
+    <t>TC09</t>
+  </si>
+  <si>
+    <t>Detect emotion</t>
+  </si>
+  <si>
+    <t>1. Open attendance page</t>
+  </si>
+  <si>
+    <t>2. Mark attendance for logged in user.</t>
+  </si>
+  <si>
+    <t>While marking attendance , it should detect emotion of face. (Pass)</t>
+  </si>
+  <si>
+    <t>TC10</t>
+  </si>
+  <si>
+    <t>Detect correct emotion</t>
+  </si>
+  <si>
+    <t>1. Mark attendance for logged in user.</t>
+  </si>
+  <si>
+    <t>Emotion detection can mark incorrect emotion based on Webcam quality and different operation system (can Fail)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -543,21 +578,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="37.875" customWidth="1"/>
-    <col min="3" max="3" width="53.875" customWidth="1"/>
-    <col min="4" max="4" width="106.875" customWidth="1"/>
+    <col min="2" max="2" width="37.8984375" customWidth="1"/>
+    <col min="3" max="3" width="53.8984375" customWidth="1"/>
+    <col min="4" max="4" width="106.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -571,7 +606,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -582,157 +617,195 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75">
-      <c r="C3" s="1" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75">
-      <c r="C4" s="1" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" t="s">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75">
-      <c r="C6" s="1" t="s">
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
+      <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
+      <c r="G7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75">
-      <c r="C8" s="1" t="s">
+      <c r="B9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
+      <c r="C9" t="s">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>22</v>
       </c>
-      <c r="D9" t="s">
+      <c r="B11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75">
-      <c r="C10" s="1" t="s">
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
+      <c r="B13" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C13" t="s">
         <v>26</v>
       </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="D13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75">
-      <c r="C12" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C13" t="s">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>30</v>
       </c>
-      <c r="D13" t="s">
+      <c r="B16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="15.75">
-      <c r="C14" s="1" t="s">
+      <c r="C16" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75">
-      <c r="C15" s="1" t="s">
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>34</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>35</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
         <v>36</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="15.75">
-      <c r="C17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="F18" t="s">
         <v>40</v>
       </c>
-      <c r="C18" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <ignoredErrors>
-    <ignoredError sqref="A18:C18 A1:D1 A2:B2 D2 A5:B5 D5 A7:B7 A9:B9 D9 A11:B11 D11 A13:B13 D13 A16:B16" numberStoredAsText="1"/>
+    <ignoredError sqref="A18:C18 A1:D1 A2:B2 A5:B5 A7:B7 A9:B9 A11:B11 A13:B13 D13 A16:B16" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>